<commit_message>
Added more kernel improvements
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,31 @@
           <t>CUDA Time Numba naive</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>CUDA Time Numba GMC</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>CUDA Time Numba SMC</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CUDA Time naive</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>CUDA Time Global Memory Coalescing</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>CUDA Time Shared Memory Caching</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -470,13 +495,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.092190027236938</v>
+        <v>1.06029200553894</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3440797328948975</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.6060397624969482</v>
+        <v>0.3211402893066406</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>0.5894157886505127</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.2652904987335205</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.4007976055145264</v>
       </c>
     </row>
     <row r="3">
@@ -489,13 +523,190 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.093238115310669</v>
+        <v>1.062727451324463</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3400907516479492</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.6016008853912354</v>
+        <v>0.3201684951782227</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>0.5928997993469238</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.2629694938659668</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.4061641693115234</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Trial 3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.5591764450073242</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1635632514953613</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>0.3131606578826904</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.1087098121643066</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.1495988368988037</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Trial 4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5570096969604492</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1581416130065918</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>0.3169970512390137</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.1077165603637695</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.1471126079559326</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Trial 5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5584828853607178</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1705427169799805</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>0.3161542415618896</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.1067156791687012</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.1486248970031738</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Trial 6</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5551903247833252</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1615891456604004</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>0.3157603740692139</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.1097064018249512</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.149599552154541</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Trial 7</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.5555508136749268</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.1625645160675049</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>0.2972052097320557</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.1107287406921387</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.1565570831298828</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Trial 8</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.5511729717254639</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.16054368019104</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>0.319221019744873</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.105689525604248</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.1506044864654541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more CUDA hardware info and ran some trials.
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,35 +456,20 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>CUDA Time Numba naive</t>
+          <t>CUDA Time naive</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>CUDA Time Numba GMC</t>
+          <t>CUDA Time Global Memory Coalescing</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>CUDA Time Numba SMC</t>
+          <t>CUDA Time Shared Memory Caching</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>CUDA Time naive</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>CUDA Time Global Memory Coalescing</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>CUDA Time Shared Memory Caching</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>CUDA Time Vectorized</t>
         </is>
@@ -497,27 +482,26 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.1835100650787354</v>
       </c>
       <c r="C2" t="n">
-        <v>1.06029200553894</v>
+        <v>0.3670196533203125</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3211402893066406</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+        <v>0.1396265029907227</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.2782862186431885</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.1037919521331787</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.1685497760772705</v>
+      </c>
       <c r="H2" t="n">
-        <v>0.5894157886505127</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.2652904987335205</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.4007976055145264</v>
-      </c>
-      <c r="K2" t="inlineStr"/>
+        <v>0.007978200912475586</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -526,27 +510,26 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1.27190637588501</v>
       </c>
       <c r="C3" t="n">
-        <v>1.062727451324463</v>
+        <v>0.3680684566497803</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3201684951782227</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+        <v>0.1385462284088135</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.2707839012145996</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.09776902198791504</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1651246547698975</v>
+      </c>
       <c r="H3" t="n">
-        <v>0.5928997993469238</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.2629694938659668</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.4061641693115234</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
+        <v>0.006981134414672852</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -555,27 +538,26 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>10.34896802902222</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5591764450073242</v>
+        <v>0.3919186592102051</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1635632514953613</v>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+        <v>0.1615924835205078</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.2872602939605713</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.09973311424255371</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.1665551662445068</v>
+      </c>
       <c r="H4" t="n">
-        <v>0.3131606578826904</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.1087098121643066</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.1495988368988037</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
+        <v>0.007978439331054688</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -584,27 +566,26 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>81.88474631309509</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5570096969604492</v>
+        <v>0.5326075553894043</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1581416130065918</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+        <v>0.1595427989959717</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.2802505493164062</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.1057174205780029</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1805171966552734</v>
+      </c>
       <c r="H5" t="n">
-        <v>0.3169970512390137</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.1077165603637695</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.1471126079559326</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
+        <v>0.01595759391784668</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -613,27 +594,26 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>658.4106531143188</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5584828853607178</v>
+        <v>2.447493553161621</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1705427169799805</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+        <v>0.3580436706542969</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.3258554935455322</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.1446144580841064</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.2114338874816895</v>
+      </c>
       <c r="H6" t="n">
-        <v>0.3161542415618896</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.1067156791687012</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.1486248970031738</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
+        <v>0.04986810684204102</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -642,144 +622,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>5501.495353937149</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5551903247833252</v>
+        <v>16.37320613861084</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1615891456604004</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+        <v>1.764312267303467</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.119626760482788</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3161547183990479</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.3909842967987061</v>
+      </c>
       <c r="H7" t="n">
-        <v>0.3157603740692139</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.1097064018249512</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.149599552154541</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Trial 7</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.5555508136749268</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.1625645160675049</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>0.2972052097320557</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.1107287406921387</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.1565570831298828</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Trial 8</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.5511729717254639</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.16054368019104</v>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
-        <v>0.319221019744873</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.105689525604248</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.1506044864654541</v>
-      </c>
-      <c r="K9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Trial 9</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>88.404221534729</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.8171510696411133</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.1856162548065186</v>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
-        <v>1.064274311065674</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.1146929264068604</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.1546413898468018</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Trial 10</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>80.63011026382446</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.5814464092254639</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.1591329574584961</v>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="n">
-        <v>0.2903285026550293</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.1057174205780029</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.1436154842376709</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.01398468017578125</v>
+        <v>0.2032253742218018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran all proposed trials when possible
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -671,6 +671,314 @@
         <v>10.46019577980042</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Trial 8</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>14.3907253742218</v>
+      </c>
+      <c r="F9" t="n">
+        <v>13.88457727432251</v>
+      </c>
+      <c r="G9" t="n">
+        <v>16.58563923835754</v>
+      </c>
+      <c r="H9" t="n">
+        <v>13.90225052833557</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Trial 9</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>14.10806488990784</v>
+      </c>
+      <c r="F10" t="n">
+        <v>13.98515152931213</v>
+      </c>
+      <c r="G10" t="n">
+        <v>30.99015283584595</v>
+      </c>
+      <c r="H10" t="n">
+        <v>13.90586185455322</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Trial 10</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>14.1343719959259</v>
+      </c>
+      <c r="F11" t="n">
+        <v>14.00995993614197</v>
+      </c>
+      <c r="G11" t="n">
+        <v>63.32477641105652</v>
+      </c>
+      <c r="H11" t="n">
+        <v>13.89554309844971</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Trial 11</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>14.10972428321838</v>
+      </c>
+      <c r="F12" t="n">
+        <v>13.98259258270264</v>
+      </c>
+      <c r="G12" t="n">
+        <v>137.5324246883392</v>
+      </c>
+      <c r="H12" t="n">
+        <v>13.90477609634399</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Trial 12</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7.791940450668335</v>
+      </c>
+      <c r="F13" t="n">
+        <v>7.603684425354004</v>
+      </c>
+      <c r="G13" t="n">
+        <v>4.725376844406128</v>
+      </c>
+      <c r="H13" t="n">
+        <v>7.510883331298828</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Trial 13</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>7.796133756637573</v>
+      </c>
+      <c r="F14" t="n">
+        <v>7.608644247055054</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.80347752571106</v>
+      </c>
+      <c r="H14" t="n">
+        <v>7.557884216308594</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Trial 14</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>7.748147487640381</v>
+      </c>
+      <c r="F15" t="n">
+        <v>7.62830924987793</v>
+      </c>
+      <c r="G15" t="n">
+        <v>18.12826251983643</v>
+      </c>
+      <c r="H15" t="n">
+        <v>7.569580793380737</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Trial 15</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>7.83071756362915</v>
+      </c>
+      <c r="F16" t="n">
+        <v>7.661117315292358</v>
+      </c>
+      <c r="G16" t="n">
+        <v>41.8465895652771</v>
+      </c>
+      <c r="H16" t="n">
+        <v>7.605157136917114</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Trial 16</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10.75392031669617</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10.64612007141113</v>
+      </c>
+      <c r="G17" t="n">
+        <v>11.42532658576965</v>
+      </c>
+      <c r="H17" t="n">
+        <v>10.54792332649231</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Trial 17</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10.74261164665222</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10.65383958816528</v>
+      </c>
+      <c r="G18" t="n">
+        <v>28.15839242935181</v>
+      </c>
+      <c r="H18" t="n">
+        <v>10.49790549278259</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Trial 18</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>21.34992527961731</v>
+      </c>
+      <c r="F19" t="n">
+        <v>21.14037585258484</v>
+      </c>
+      <c r="G19" t="n">
+        <v>21.50210118293762</v>
+      </c>
+      <c r="H19" t="n">
+        <v>21.14603114128113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Re-ran failed trials with just vectorized kernel since that should help deal with alignment.
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -979,6 +979,146 @@
         <v>21.14603114128113</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Trial 19</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10.46670031547546</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10.3735408782959</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>10.28624629974365</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Trial 20</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10.47215461730957</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10.36481404304504</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>10.29764723777771</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Trial 21</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>21.09299921989441</v>
+      </c>
+      <c r="F22" t="n">
+        <v>20.84064340591431</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>20.98466849327087</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Trial 22</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>21.25983667373657</v>
+      </c>
+      <c r="F23" t="n">
+        <v>20.84869337081909</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>20.91546201705933</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Trial 23</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>21.23253870010376</v>
+      </c>
+      <c r="F24" t="n">
+        <v>20.91148519515991</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>20.95027732849121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Ran a couple more profiling trials on interesting previous cases. Cleaned up a bit.
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1119,6 +1119,146 @@
         <v>20.95027732849121</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Trial 24</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>136.4511978626251</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Trial 25</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>4.844620943069458</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Trial 26</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>41.60684609413147</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Trial 27</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>7.688782691955566</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Trial 28</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>21.1106321811676</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Setting up for MKL and cuBLAS a little bit.
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1259,6 +1259,34 @@
         <v>21.1106321811676</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Trial 29</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>88.65517687797546</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.721221923828125</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.1725394725799561</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.2868828773498535</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.1107616424560547</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.1794347763061523</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.01595711708068848</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fully implemented CuBLAS and MKL and re-ran matrix size trials with the optimized libraries for baseline.
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,16 @@
           <t>CUDA Time Vectorized</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>MKL Time</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>CuBLAS Time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -502,6 +512,8 @@
       <c r="H2" t="n">
         <v>0.007978200912475586</v>
       </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -530,6 +542,8 @@
       <c r="H3" t="n">
         <v>0.006981134414672852</v>
       </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -558,6 +572,8 @@
       <c r="H4" t="n">
         <v>0.007978439331054688</v>
       </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -586,6 +602,8 @@
       <c r="H5" t="n">
         <v>0.01595759391784668</v>
       </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -614,6 +632,8 @@
       <c r="H6" t="n">
         <v>0.04986810684204102</v>
       </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -642,6 +662,8 @@
       <c r="H7" t="n">
         <v>0.2032253742218018</v>
       </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -670,6 +692,8 @@
       <c r="H8" t="n">
         <v>10.46019577980042</v>
       </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -698,6 +722,8 @@
       <c r="H9" t="n">
         <v>13.90225052833557</v>
       </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -726,6 +752,8 @@
       <c r="H10" t="n">
         <v>13.90586185455322</v>
       </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -754,6 +782,8 @@
       <c r="H11" t="n">
         <v>13.89554309844971</v>
       </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -782,6 +812,8 @@
       <c r="H12" t="n">
         <v>13.90477609634399</v>
       </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -810,6 +842,8 @@
       <c r="H13" t="n">
         <v>7.510883331298828</v>
       </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -838,6 +872,8 @@
       <c r="H14" t="n">
         <v>7.557884216308594</v>
       </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -866,6 +902,8 @@
       <c r="H15" t="n">
         <v>7.569580793380737</v>
       </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -894,6 +932,8 @@
       <c r="H16" t="n">
         <v>7.605157136917114</v>
       </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -922,6 +962,8 @@
       <c r="H17" t="n">
         <v>10.54792332649231</v>
       </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -950,6 +992,8 @@
       <c r="H18" t="n">
         <v>10.49790549278259</v>
       </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -978,6 +1022,8 @@
       <c r="H19" t="n">
         <v>21.14603114128113</v>
       </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1006,6 +1052,8 @@
       <c r="H20" t="n">
         <v>10.28624629974365</v>
       </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1034,6 +1082,8 @@
       <c r="H21" t="n">
         <v>10.29764723777771</v>
       </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1062,6 +1112,8 @@
       <c r="H22" t="n">
         <v>20.98466849327087</v>
       </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1090,6 +1142,8 @@
       <c r="H23" t="n">
         <v>20.91546201705933</v>
       </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1118,6 +1172,8 @@
       <c r="H24" t="n">
         <v>20.95027732849121</v>
       </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1146,6 +1202,8 @@
       <c r="H25" t="n">
         <v>0</v>
       </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1174,6 +1232,8 @@
       <c r="H26" t="n">
         <v>0</v>
       </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1202,6 +1262,8 @@
       <c r="H27" t="n">
         <v>0</v>
       </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1230,6 +1292,8 @@
       <c r="H28" t="n">
         <v>7.688782691955566</v>
       </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1258,6 +1322,8 @@
       <c r="H29" t="n">
         <v>21.1106321811676</v>
       </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1285,6 +1351,246 @@
       </c>
       <c r="H30" t="n">
         <v>0.01595711708068848</v>
+      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Trial 30</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.3082060813903809</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.002991914749145508</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.1581034660339355</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Trial 31</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.293776273727417</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.002990961074829102</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.1805171966552734</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Trial 32</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.3042478561401367</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.003988981246948242</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.1695470809936523</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Trial 33</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.3093512058258057</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.004986286163330078</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.1785213947296143</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Trial 34</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.3185737133026123</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.0139617919921875</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.183509349822998</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Trial 35</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.5135586261749268</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.08676838874816895</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.1924829483032227</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Trial 36</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>10.25245118141174</v>
+      </c>
+      <c r="I37" t="n">
+        <v>4.482025146484375</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.8058481216430664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran two larger matrix size sets
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1593,6 +1593,74 @@
         <v>0.8058481216430664</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Trial 37</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>80.53076314926147</v>
+      </c>
+      <c r="F38" t="n">
+        <v>81.70234942436218</v>
+      </c>
+      <c r="G38" t="n">
+        <v>86.79865407943726</v>
+      </c>
+      <c r="H38" t="n">
+        <v>81.36654353141785</v>
+      </c>
+      <c r="I38" t="n">
+        <v>36.32433462142944</v>
+      </c>
+      <c r="J38" t="n">
+        <v>3.009976148605347</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Trial 38</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>663.6075005531311</v>
+      </c>
+      <c r="F39" t="n">
+        <v>666.0170459747314</v>
+      </c>
+      <c r="G39" t="n">
+        <v>683.7945878505707</v>
+      </c>
+      <c r="H39" t="n">
+        <v>664.8327276706696</v>
+      </c>
+      <c r="I39" t="n">
+        <v>289.1930079460144</v>
+      </c>
+      <c r="J39" t="n">
+        <v>14.67776441574097</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>